<commit_message>
Phew, glad noone reads these.
</commit_message>
<xml_diff>
--- a/MS_M365.xlsx
+++ b/MS_M365.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26105"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7c26969d82fe7094/Dokumenty/Personal/personalNotes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="790" documentId="11_AD4D80C4656A4B7AC02E74B03BDC76585BDEDD86" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AF2CDA29-1355-43D8-8DC8-4D55C246225E}"/>
+  <xr:revisionPtr revIDLastSave="791" documentId="11_AD4D80C4656A4B7AC02E74B03BDC76585BDEDD86" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4B50FA28-B349-49FE-B3F9-1D7FEE7A1B8C}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" firstSheet="2" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cloud Concepts" sheetId="11" r:id="rId1"/>
@@ -4172,6 +4172,9 @@
     <t>Správní jednotky (Administrative Units)</t>
   </si>
   <si>
+    <t>portal.microsoft.com -&gt; Role -&gt; Správní jednotky</t>
+  </si>
+  <si>
     <t>- Pro administrátory představují role prostředek k přidělování administrátorských oprávnění ve vašem prostředí Azure/Microsoft 365</t>
   </si>
   <si>
@@ -4188,9 +4191,6 @@
   </si>
   <si>
     <t>- Administrativní jednotky omezují oprávnění v roli na jakoukoli část vaší organizace, kterou definujete</t>
-  </si>
-  <si>
-    <t>portal.microsoft.com -&gt; Role -&gt; Správní jednotky</t>
   </si>
   <si>
     <t>- Můžete například použít administrativní jednotky k delegování role administrátora Helpdesku na regionální specialisty podpory, takže uživatelé mohou spravovat uživatele pouze v regionu, který podporují.</t>
@@ -7335,6 +7335,12 @@
     <xf numFmtId="0" fontId="47" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="28" fillId="2" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="22" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -7352,12 +7358,6 @@
     </xf>
     <xf numFmtId="0" fontId="17" fillId="20" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="2" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -8178,7 +8178,7 @@
   </sheetPr>
   <dimension ref="A1:AA1088"/>
   <sheetViews>
-    <sheetView topLeftCell="A163" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A171" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
@@ -8190,7 +8190,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A1" s="177" t="s">
+      <c r="A1" s="171" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="200"/>
@@ -8384,20 +8384,20 @@
       <c r="J7" s="124"/>
       <c r="K7" s="124"/>
       <c r="L7" s="124"/>
-      <c r="M7" s="178" t="s">
+      <c r="M7" s="172" t="s">
         <v>4</v>
       </c>
-      <c r="N7" s="178"/>
-      <c r="O7" s="178"/>
-      <c r="P7" s="178" t="s">
+      <c r="N7" s="172"/>
+      <c r="O7" s="172"/>
+      <c r="P7" s="172" t="s">
         <v>5</v>
       </c>
-      <c r="Q7" s="178"/>
-      <c r="R7" s="178" t="s">
+      <c r="Q7" s="172"/>
+      <c r="R7" s="172" t="s">
         <v>6</v>
       </c>
-      <c r="S7" s="178"/>
-      <c r="T7" s="178"/>
+      <c r="S7" s="172"/>
+      <c r="T7" s="172"/>
       <c r="U7" s="124"/>
       <c r="V7" s="124"/>
       <c r="W7" s="124"/>
@@ -8539,20 +8539,20 @@
       <c r="A13" s="154" t="s">
         <v>15</v>
       </c>
-      <c r="M13" s="178" t="s">
+      <c r="M13" s="172" t="s">
         <v>16</v>
       </c>
-      <c r="N13" s="178"/>
-      <c r="O13" s="178"/>
-      <c r="P13" s="178" t="s">
+      <c r="N13" s="172"/>
+      <c r="O13" s="172"/>
+      <c r="P13" s="172" t="s">
         <v>5</v>
       </c>
-      <c r="Q13" s="178"/>
-      <c r="R13" s="178" t="s">
+      <c r="Q13" s="172"/>
+      <c r="R13" s="172" t="s">
         <v>17</v>
       </c>
-      <c r="S13" s="178"/>
-      <c r="T13" s="178"/>
+      <c r="S13" s="172"/>
+      <c r="T13" s="172"/>
       <c r="U13" s="124"/>
       <c r="V13" s="124"/>
       <c r="W13" s="124"/>
@@ -8797,7 +8797,7 @@
       <c r="C27" s="124"/>
       <c r="D27" s="124"/>
       <c r="E27" s="124"/>
-      <c r="H27" s="173" t="s">
+      <c r="H27" s="175" t="s">
         <v>28</v>
       </c>
       <c r="J27" s="133" t="s">
@@ -9062,7 +9062,7 @@
       <c r="AA35" s="124"/>
     </row>
     <row r="36" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A36" s="174" t="s">
+      <c r="A36" s="176" t="s">
         <v>40</v>
       </c>
       <c r="B36" s="210"/>
@@ -9119,7 +9119,7 @@
       <c r="N37" s="124"/>
       <c r="O37" s="124"/>
       <c r="P37" s="124"/>
-      <c r="Q37" s="175" t="s">
+      <c r="Q37" s="177" t="s">
         <v>46</v>
       </c>
       <c r="R37" s="208"/>
@@ -9191,7 +9191,7 @@
       <c r="AA39" s="124"/>
     </row>
     <row r="40" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A40" s="176" t="s">
+      <c r="A40" s="178" t="s">
         <v>49</v>
       </c>
       <c r="B40" s="211"/>
@@ -9206,7 +9206,7 @@
       <c r="I40" s="124"/>
       <c r="J40" s="124"/>
       <c r="K40" s="124"/>
-      <c r="L40" s="175" t="s">
+      <c r="L40" s="177" t="s">
         <v>51</v>
       </c>
       <c r="M40" s="208"/>
@@ -9312,7 +9312,7 @@
       <c r="AA43" s="124"/>
     </row>
     <row r="44" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A44" s="171" t="s">
+      <c r="A44" s="173" t="s">
         <v>59</v>
       </c>
       <c r="B44" s="212"/>
@@ -9365,7 +9365,7 @@
       <c r="N45" s="124"/>
       <c r="O45" s="124"/>
       <c r="P45" s="138"/>
-      <c r="Q45" s="172" t="s">
+      <c r="Q45" s="174" t="s">
         <v>64</v>
       </c>
       <c r="R45" s="208"/>
@@ -39397,13 +39397,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A1:H4"/>
-    <mergeCell ref="M7:O7"/>
-    <mergeCell ref="P7:Q7"/>
-    <mergeCell ref="R7:T7"/>
-    <mergeCell ref="M13:O13"/>
-    <mergeCell ref="P13:Q13"/>
-    <mergeCell ref="R13:T13"/>
     <mergeCell ref="A44:C46"/>
     <mergeCell ref="Q45:T46"/>
     <mergeCell ref="H27:H31"/>
@@ -39412,6 +39405,13 @@
     <mergeCell ref="Q37:T38"/>
     <mergeCell ref="A40:C42"/>
     <mergeCell ref="L40:O41"/>
+    <mergeCell ref="A1:H4"/>
+    <mergeCell ref="M7:O7"/>
+    <mergeCell ref="P7:Q7"/>
+    <mergeCell ref="R7:T7"/>
+    <mergeCell ref="M13:O13"/>
+    <mergeCell ref="P13:Q13"/>
+    <mergeCell ref="R13:T13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -39426,8 +39426,8 @@
   </sheetPr>
   <dimension ref="A1:T511"/>
   <sheetViews>
-    <sheetView topLeftCell="A211" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J231" sqref="J231"/>
+    <sheetView tabSelected="1" topLeftCell="A360" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O372" sqref="O372"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15"/>
@@ -42423,31 +42423,31 @@
       </c>
       <c r="L372" s="9"/>
       <c r="M372" s="9"/>
+      <c r="O372" s="15" t="s">
+        <v>765</v>
+      </c>
     </row>
     <row r="373" spans="1:16">
       <c r="A373" s="2" t="s">
-        <v>765</v>
+        <v>766</v>
       </c>
       <c r="K373" s="2" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
     </row>
     <row r="374" spans="1:16">
       <c r="A374" s="2" t="s">
-        <v>767</v>
+        <v>768</v>
       </c>
       <c r="K374" s="2" t="s">
-        <v>768</v>
+        <v>769</v>
       </c>
     </row>
     <row r="375" spans="1:16">
       <c r="A375" s="2" t="s">
-        <v>769</v>
+        <v>770</v>
       </c>
       <c r="K375" s="2" t="s">
-        <v>770</v>
-      </c>
-      <c r="O375" s="15" t="s">
         <v>771</v>
       </c>
     </row>
@@ -43209,7 +43209,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06AF4BC9-33CC-4F36-BF08-DBC4CC0FC524}">
   <dimension ref="A1:Q153"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>

</xml_diff>